<commit_message>
10.11.2024 - wykonanie mini pomocy oraz szablonów plików do importu
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6391392-1A42-4648-AD54-4C2BAE8439B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78EA5E5-40C0-406F-983A-2588DF964D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="2580" windowWidth="25170" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Lp</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Sprawdzić jak nazywa się zakładka w Excelu z danymi tak by pobrać dane i by nie generowało to błędów programu</t>
+  </si>
+  <si>
+    <t>dodać ramki do zestawień jeszcze. Postarać się sformatować całość</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +480,7 @@
     <col min="2" max="2" width="20.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="112.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -498,11 +502,11 @@
       </c>
       <c r="G1">
         <f>SUM(D2:D54)</f>
-        <v>300</v>
+        <v>575</v>
       </c>
       <c r="H1">
         <f>G1/F1</f>
-        <v>13.043478260869565</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -513,7 +517,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -524,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -788,7 +795,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
24.11.2024 - kilka poprawek, powtórne importy, dodawanie w jakości itp
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78EA5E5-40C0-406F-983A-2588DF964D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1916BD3A-4E5F-4AE5-A617-1D4FAEF9C572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2580" windowWidth="25170" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="135" windowWidth="23685" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Lp</t>
   </si>
@@ -142,16 +145,85 @@
   </si>
   <si>
     <t>dodać ramki do zestawień jeszcze. Postarać się sformatować całość</t>
+  </si>
+  <si>
+    <t>Dostosować szerokości kolumn w zestawieniach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Możliwość powtórnego wprowadzenia danych (skasowanie poprzednich i import nowych) </t>
+  </si>
+  <si>
+    <t>Pracownicy</t>
+  </si>
+  <si>
+    <t>Błędy produkcji</t>
+  </si>
+  <si>
+    <t>Nieobecności</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Raportownie (szczeg)</t>
+  </si>
+  <si>
+    <t>Raportownie (total)</t>
+  </si>
+  <si>
+    <t>poprawa raportu z danymi dla pracowników. Formatowanie komórek, wyrównanie, przedstawienie danych</t>
+  </si>
+  <si>
+    <t>Wprowadzića tą metodę do innych okien, prawdopodobnie wszystkich</t>
+  </si>
+  <si>
+    <t>Dodać możliwość kasowania jednego rekordu</t>
+  </si>
+  <si>
+    <t>Sprawdzić poprawność filtrowania danych w grupach roboczych. Są różnie zapisanete same dane np. "3013+3015" i "3013 + 3015"</t>
+  </si>
+  <si>
+    <t>Odkomentować zapis, dodać wykluczenie dodanych już grup roboczych i lokalizacji</t>
+  </si>
+  <si>
+    <t>Instalator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stworzyć wersję .exe oraz doprowadzić by obrazy wyświetlały się i były pobierane z właściwej lokalizacji. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -188,6 +260,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -468,22 +543,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="20.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="112.5703125" customWidth="1"/>
+    <col min="3" max="3" width="115.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,17 +573,17 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1">
-        <f>COUNTA(C2:C186)</f>
-        <v>23</v>
-      </c>
-      <c r="G1">
-        <f>SUM(D2:D54)</f>
-        <v>575</v>
-      </c>
-      <c r="H1">
+      <c r="F1" s="5">
+        <f>COUNTA(C2:C200)</f>
+        <v>36</v>
+      </c>
+      <c r="G1" s="5">
+        <f>SUM(D2:D200)</f>
+        <v>2055</v>
+      </c>
+      <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>25</v>
+        <v>57.083333333333336</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -661,7 +738,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -675,7 +755,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -692,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -706,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -717,10 +797,13 @@
         <v>25</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -734,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -745,10 +828,10 @@
         <v>28</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -762,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -776,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -787,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -798,58 +881,221 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <autoFilter ref="A1:D34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="D2:D98">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -864,6 +1110,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -878,7 +1125,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D2:D29</xm:sqref>
+          <xm:sqref>D2:D98</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
01.11.2024 - korekty i poprawki funkcjonalnosci
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1916BD3A-4E5F-4AE5-A617-1D4FAEF9C572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC79C9B-B7AB-4B62-9A8F-3BC883D69A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="135" windowWidth="23685" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="480" windowWidth="26670" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz1" sheetId="2" r:id="rId2"/>
+    <sheet name="Arkusz2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$34</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Lp</t>
   </si>
@@ -190,6 +191,33 @@
   </si>
   <si>
     <t xml:space="preserve">Stworzyć wersję .exe oraz doprowadzić by obrazy wyświetlały się i były pobierane z właściwej lokalizacji. </t>
+  </si>
+  <si>
+    <t>sprawdziće sumę liderów i instruktorów. Suma całości jest 0 jeśli jakość jest 0 - to złe rozwiązanie</t>
+  </si>
+  <si>
+    <t>import danych</t>
+  </si>
+  <si>
+    <t>wszystkie miejsca gdzie dane tabelaryczne zbpisywane są ręcznie należy wprowadzić mechanizm sprawdzania czy wpisy się nie powielają. Najlepiej będzie jeśli taki import będzie blokowany.</t>
+  </si>
+  <si>
+    <t>Wprowadzić paski postępu. Powinno być widać że program pracuje</t>
+  </si>
+  <si>
+    <t>Zapis wyliczeń kasuje istniejące już dane zarówno dla produkcji jak i dla magazynu</t>
+  </si>
+  <si>
+    <t>listopad</t>
+  </si>
+  <si>
+    <t>Ustawienia magazyn</t>
+  </si>
+  <si>
+    <t>Dodać edycję pracowników. Najlepiej klikając 2x by otwierał się formularz lub zaznaczając pozycję i klikając przycisk edycji</t>
+  </si>
+  <si>
+    <t>Dodać edycję parametrów i wytycznych</t>
   </si>
 </sst>
 </file>
@@ -249,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +291,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -546,8 +577,8 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,15 +606,15 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C200)</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D200)</f>
-        <v>2055</v>
+        <v>2205</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>57.083333333333336</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -814,7 +845,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,7 +873,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,30 +1098,78 @@
       <c r="A38" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
+      <c r="C41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
+      <c r="B42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1151,4 +1230,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A7E361-4F26-4265-A7D1-8C63235527B5}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>100</v>
+      </c>
+      <c r="D1">
+        <v>75</v>
+      </c>
+      <c r="F1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <f>(B2/4)*3</f>
+        <v>14.25</v>
+      </c>
+      <c r="F2">
+        <f>B2/2</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
02.11.2024 - Poprawki do importu danych
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC79C9B-B7AB-4B62-9A8F-3BC883D69A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B48878-98D7-4155-95BA-D95C14EE8C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="375" yWindow="480" windowWidth="26670" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>Lp</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Dodać edycję parametrów i wytycznych</t>
+  </si>
+  <si>
+    <t>Kasowanie wpisów podczas powtórnego importu</t>
+  </si>
+  <si>
+    <t>Dodać możliwość wprowadzania przecinka i zamiany go na kropkę w czasie zapisu</t>
   </si>
 </sst>
 </file>
@@ -574,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +612,7 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C200)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D200)</f>
@@ -614,7 +620,7 @@
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>52.5</v>
+        <v>50.113636363636367</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1169,6 +1175,34 @@
         <v>58</v>
       </c>
       <c r="D43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
29.12.2024 - Optymalizacja formularzy - poprawa tworzenia tabel w formularzach. Uproszczenie i ujednolicenie kodu.
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B48878-98D7-4155-95BA-D95C14EE8C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B1A402-8D5A-4862-AD03-80D8164C48EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="480" windowWidth="26670" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="2010" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Lp</t>
   </si>
@@ -220,10 +220,58 @@
     <t>Dodać edycję parametrów i wytycznych</t>
   </si>
   <si>
-    <t>Kasowanie wpisów podczas powtórnego importu</t>
-  </si>
-  <si>
-    <t>Dodać możliwość wprowadzania przecinka i zamiany go na kropkę w czasie zapisu</t>
+    <t xml:space="preserve">wyliczenia pracowników </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyliczany jest Direct i Indirect godzinowy a powinien być procentowy. </t>
+  </si>
+  <si>
+    <t>Po wyliczeniu procentowym mogą pojawić się wartości ujemne co może powodować wartości NULL. Wartości te wywalają program. Zamienić ujemne wartości lub NULL na 0</t>
+  </si>
+  <si>
+    <t>Wyliczenia mag</t>
+  </si>
+  <si>
+    <t>Gdy wśród pracowników jest obcokrajowiec to nie ma kodu z Enova. Przez to osoba nie jest zapisywana do pliku do eksportu. Należy dodać warunek by kod był zastąpiony na 0 w szędzie gdzie może pojawić się obcokrajowiec.</t>
+  </si>
+  <si>
+    <t>Nieobecności - import cyfr po przecinku powoduje błąd i pomija dany wiersz. Należy odczytać te dane, zaokrąglić do INT i zaimportować</t>
+  </si>
+  <si>
+    <t>zaokrąglone w dół na korzyść pracowników</t>
+  </si>
+  <si>
+    <t>nie wyelininowane są jeszcze wartości ujemne. Wartości NULL są zrobione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edycja danych. </t>
+  </si>
+  <si>
+    <t>Na przykładzie formsa błędów magazynowych sprawdzić możliwość dodania przycisku do czyszczenia danych z bieżącego misiąca po to by je wczytać ponownie. Przycisk czyszczenia jest nieaktywny jeśli nie ma danych, natoniast przycisk importu jest nieaktywny jeśli są zaimportowane dane.</t>
+  </si>
+  <si>
+    <t>Ustawienia</t>
+  </si>
+  <si>
+    <t>Zmienić formularz do importu i obsługi dni wolnych od pracy. Dostosować do innych formularzy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodać szablon do wprowadzania dni wolnych w roku kalendarzowym </t>
+  </si>
+  <si>
+    <t>Znaleźć sposób na odświerzanie formsa jeśli dodana jest edycja komórek. W tej chwili działa albo edycja abo odświeżanie.</t>
+  </si>
+  <si>
+    <t>zbudować forms Edycja Lider &lt;=&gt; WC</t>
+  </si>
+  <si>
+    <t>zbudować forms Edycja Liderzy</t>
+  </si>
+  <si>
+    <t>zbudować forms Edycja Linie</t>
+  </si>
+  <si>
+    <t>zbudować forms Edycja Lokalizacje</t>
   </si>
 </sst>
 </file>
@@ -283,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -299,6 +347,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,11 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,16 +662,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="5">
-        <f>COUNTA(C2:C200)</f>
-        <v>44</v>
+        <f>COUNTA(C2:C199)</f>
+        <v>54</v>
       </c>
       <c r="G1" s="5">
-        <f>SUM(D2:D200)</f>
-        <v>2205</v>
+        <f>SUM(D2:D199)</f>
+        <v>2655</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>50.113636363636367</v>
+        <v>49.166666666666664</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1030,7 +1081,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1044,7 +1095,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1058,7 +1109,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1072,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1086,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1100,7 +1151,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1111,10 +1162,10 @@
         <v>50</v>
       </c>
       <c r="D38" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1128,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1139,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1147,10 +1198,10 @@
         <v>54</v>
       </c>
       <c r="D41" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1164,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1178,38 +1229,182 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D44" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D45" s="3">
+        <v>50</v>
+      </c>
+      <c r="E45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="3">
+        <v>100</v>
+      </c>
+      <c r="E47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="D2:D98">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="D2:D97">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1238,7 +1433,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D2:D98</xm:sqref>
+          <xm:sqref>D2:D97</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
01.01.2025 - Dodanie sortowania oraz wyrównania danych w tabelach
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B1A402-8D5A-4862-AD03-80D8164C48EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740921B1-437A-4B31-8B43-0B96ADF828E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="2010" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -634,8 +634,8 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,11 +667,11 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
-        <v>2655</v>
+        <v>3055</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>49.166666666666664</v>
+        <v>56.574074074074076</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
08.01.2025 - Poprawa błędów i niedociągnięć ostatniej aktualizacji. Przywrócenie funkcjonalności przycisków.
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740921B1-437A-4B31-8B43-0B96ADF828E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EE054E-CC54-4C0A-A592-9BF93206C9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2010" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>Lp</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>zbudować forms Edycja Lokalizacje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChatGPT, przy okazji eliminacji liczb dziesiętnych przy wczytywaniu nieobecności, pokazuje inną metodę zapisu do bazy z pliku Excel. Sprawdzić to, przeanalizować i zastodować. </t>
+  </si>
+  <si>
+    <t>Filtrowanie danych czytanych z pliku i eliminacja liczb dziesiętnych. Zapis tylko całkowitych liczb</t>
   </si>
 </sst>
 </file>
@@ -631,11 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +669,7 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
@@ -671,7 +677,7 @@
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>56.574074074074076</v>
+        <v>54.553571428571431</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1398,6 +1404,31 @@
         <v>76</v>
       </c>
       <c r="D55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
13.01.2025 - Poprawna edycja danych w zestawieniach tabelarycznycch. Nie ma błędu podczas importu danych z pliku. Optymalizacja menu głównego. Eliminacja zbędnych zapytań do bazy.
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EE054E-CC54-4C0A-A592-9BF93206C9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C77B57-E1DF-4BA2-9BA7-BCBAA82DD27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="-13140" windowWidth="24585" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Lp</t>
   </si>
@@ -259,9 +259,6 @@
     <t xml:space="preserve">Dodać szablon do wprowadzania dni wolnych w roku kalendarzowym </t>
   </si>
   <si>
-    <t>Znaleźć sposób na odświerzanie formsa jeśli dodana jest edycja komórek. W tej chwili działa albo edycja abo odświeżanie.</t>
-  </si>
-  <si>
     <t>zbudować forms Edycja Lider &lt;=&gt; WC</t>
   </si>
   <si>
@@ -278,6 +275,15 @@
   </si>
   <si>
     <t>Filtrowanie danych czytanych z pliku i eliminacja liczb dziesiętnych. Zapis tylko całkowitych liczb</t>
+  </si>
+  <si>
+    <t>Znaleźć sposób na odświerzanie formsa jeśli dodana jest edycja komórek. Przykład - błędu magazynu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ustawienia. </t>
+  </si>
+  <si>
+    <t>Ustawienia danych w babelacg</t>
   </si>
 </sst>
 </file>
@@ -637,11 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,15 +675,15 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
-        <v>3055</v>
+        <v>3155</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>54.553571428571431</v>
+        <v>55.350877192982459</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1345,10 +1351,10 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D51" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,7 +1365,7 @@
         <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D52" s="3">
         <v>0</v>
@@ -1373,7 +1379,7 @@
         <v>69</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D53" s="3">
         <v>0</v>
@@ -1387,7 +1393,7 @@
         <v>69</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="3">
         <v>0</v>
@@ -1401,7 +1407,7 @@
         <v>69</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D55" s="3">
         <v>0</v>
@@ -1412,7 +1418,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D56" s="3">
         <v>0</v>
@@ -1426,9 +1432,23 @@
         <v>39</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D58" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
19.01.2025 - Optymalizacja kodu. Przeniesienie zapytań SQL wyliczeń do procedur w bazie danych.
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C77B57-E1DF-4BA2-9BA7-BCBAA82DD27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC3F9F7-41DF-4AC7-A87F-4C9D4DB3F2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-13140" windowWidth="24585" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="7320" windowWidth="27690" windowHeight="8085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t>Lp</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>Ustawienia danych w babelacg</t>
+  </si>
+  <si>
+    <t>wyliczenia</t>
+  </si>
+  <si>
+    <t>Stworzenie tabel tymczasowych dla wyliczeń. Ilość tabel niezbędna do zapisania wszystkich zestawień. Tabele te są tymczasowe i mogą być czyszczone zawsze podczas otwierania kolejnego miesiąca.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla WYDANIA nieobecności są indywidualne i wymagają oddzielnej procedury SQL - należy przerobić kod by ujednolicić procedurę. </t>
   </si>
 </sst>
 </file>
@@ -323,12 +332,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -343,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -363,6 +378,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -643,11 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +691,7 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
@@ -683,7 +699,7 @@
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>55.350877192982459</v>
+        <v>53.474576271186443</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1449,6 +1465,34 @@
         <v>80</v>
       </c>
       <c r="D58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1514,15 +1558,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A7E361-4F26-4265-A7D1-8C63235527B5}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>100</v>
       </c>
@@ -1533,7 +1577,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1549,7 +1593,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C3" s="7">
         <v>0</v>
       </c>
@@ -1559,6 +1603,16 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <f>R3/S3</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="9">
+        <v>0</v>
+      </c>
+      <c r="S3" s="9">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
02.02.2025 - Dalsza optymalizacja kodu. Przeniesienie zapytań SQL wyliczeń do procedur w bazie danych. Poprawa formularzy wyliczeń. Dodanie praw dostępu do programu.
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC3F9F7-41DF-4AC7-A87F-4C9D4DB3F2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E8E46D-D676-475F-912B-34312C970360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="7320" windowWidth="27690" windowHeight="8085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Arkusz2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>Lp</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t xml:space="preserve">dla WYDANIA nieobecności są indywidualne i wymagają oddzielnej procedury SQL - należy przerobić kod by ujednolicić procedurę. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla liderów dodać kolumnę WC - łatwiej będzie kontrolować kwoty </t>
+  </si>
+  <si>
+    <t>Do sprawdzenia powinno się zamykać automatycznie na teraz w momenci uruchomienia programu w nowym miesiącu.</t>
   </si>
 </sst>
 </file>
@@ -659,11 +665,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H60"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,15 +698,15 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
-        <v>3155</v>
+        <v>3305</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>53.474576271186443</v>
+        <v>55.083333333333336</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -716,7 +723,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -727,7 +734,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -738,7 +745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -749,7 +756,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -771,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -782,7 +789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -815,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -829,7 +836,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -860,7 +867,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -902,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -919,7 +926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -933,7 +940,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -983,10 +990,13 @@
         <v>32</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -997,7 +1007,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1011,7 +1021,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1025,7 +1035,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1039,7 +1049,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1053,7 +1063,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1067,7 +1077,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1081,7 +1091,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1095,7 +1105,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1109,7 +1119,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1123,7 +1133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1165,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1218,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1257,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1302,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1361,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1496,8 +1506,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="3">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D61" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="0"/>
+        <filter val="50"/>
+        <filter val="75"/>
+        <filter val="80"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="D2:D97">
     <cfRule type="dataBar" priority="2">
       <dataBar>

</xml_diff>

<commit_message>
03.02.2025 - Poprawa błędu podczas importowania raportowania zleceń
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E8E46D-D676-475F-912B-34312C970360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D5584F-AF41-4A7A-90B3-7284AF993F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
   <si>
     <t>Lp</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>Do sprawdzenia powinno się zamykać automatycznie na teraz w momenci uruchomienia programu w nowym miesiącu.</t>
+  </si>
+  <si>
+    <t>Dodać zabezpieczenie przed powtórnym zapisem. Przycisk jest już wstawiony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodać listę użytkowników w bazie danych.W tej chwili jest wpisana na sztywno w kodzie. </t>
   </si>
 </sst>
 </file>
@@ -666,11 +672,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +704,7 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
@@ -706,7 +712,7 @@
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>55.083333333333336</v>
+        <v>53.306451612903224</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1518,6 +1524,34 @@
       </c>
       <c r="D61" s="3">
         <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16.03.2025 - Zabezpieczenie przed nieświadomym wielokrotnym zapisem, Kolejność uzupełniania danych, Edycja i grupowanie kKorekty Indirect, Zmiana liczenia błędów produkcji
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D5584F-AF41-4A7A-90B3-7284AF993F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFDE86E-9477-4C8F-852A-2DE66F68ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
   <si>
     <t>Lp</t>
   </si>
@@ -301,17 +301,61 @@
     <t>Do sprawdzenia powinno się zamykać automatycznie na teraz w momenci uruchomienia programu w nowym miesiącu.</t>
   </si>
   <si>
-    <t>Dodać zabezpieczenie przed powtórnym zapisem. Przycisk jest już wstawiony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dodać listę użytkowników w bazie danych.W tej chwili jest wpisana na sztywno w kodzie. </t>
+    <t>1. Wprowadzenie zabezpieczeń co do kolejność uzupełniania danych – przykładem jest korekta IndirectWork, która musi być po imporcie Directa</t>
+  </si>
+  <si>
+    <t>1. Wprowadzenie blokady zapisu jeśli już raz zostały dane zapisane</t>
+  </si>
+  <si>
+    <t>1. Korekta indirect – możliwość dodawania importowanych danych ewentualnie kasowania wybranych danych – W tej chwili nie można dodać danych z różnych działów ponieważ jedni kasują innych.</t>
+  </si>
+  <si>
+    <t>Korekta indirect</t>
+  </si>
+  <si>
+    <t>1. Okno wyliczeń. Kilkukrotne kliknięcie przycisku Przelicz powinno kasować poprzednie przeliczenia – w tej chwili dodaje dane powielając je.</t>
+  </si>
+  <si>
+    <t>Przeniesienie transportu w Czaplinku do produkcji</t>
+  </si>
+  <si>
+    <t>Zmiana sposobu liczenia błędów. Wg nowego systemu 1 błąd to nadal 100% kwoty wyjściowej. Pozostałe parametry przesunięte o 1 w dół</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zmiana tabeli - dodanie kolumny do rozpoznania właściciela wpisów
+Dodanie zmiennej przenoszonej do formsa korekty
+rozbicie produkcji jako użytkonika na Czaplinek i Borne - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>należy zmienić parametry ikon u użytkowników</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+Dodanie zmiennej przenoszonej do formsa korekty - nowy wpis</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,8 +387,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCF8E6D"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +425,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -391,6 +468,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -672,14 +764,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60:D61"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="20.140625" style="2" customWidth="1"/>
@@ -687,9 +779,10 @@
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="115.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -704,18 +797,18 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
-        <v>3305</v>
+        <v>3705</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>53.306451612903224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56.136363636363633</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -729,7 +822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -740,7 +833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -751,7 +844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -762,7 +855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -773,7 +866,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -784,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -795,7 +888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -806,7 +899,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -817,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -828,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -842,7 +935,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -856,7 +949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -873,7 +966,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -887,7 +980,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -901,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -915,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -932,7 +1025,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -946,7 +1039,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -960,7 +1053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -974,7 +1067,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -988,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1002,7 +1095,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1013,7 +1106,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1027,7 +1120,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1041,7 +1134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1055,7 +1148,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1069,7 +1162,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1083,7 +1176,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1097,7 +1190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1111,7 +1204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1125,7 +1218,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1139,7 +1232,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1153,7 +1246,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1167,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1181,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1195,7 +1288,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1209,7 +1302,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1223,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1234,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1245,7 +1338,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1259,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1273,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1287,7 +1380,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="30">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1304,7 +1397,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="30">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1318,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" hidden="1">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1335,7 +1428,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="45">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1349,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1363,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1377,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1389,7 +1482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1403,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1417,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1431,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1445,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1456,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1470,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1484,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="30">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1498,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1512,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1526,33 +1619,96 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30">
       <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="B62" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D62" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="B63" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>87</v>
       </c>
       <c r="D63" s="3">
-        <v>0</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="60">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D64" s="3">
+        <v>100</v>
+      </c>
+      <c r="G64" s="12"/>
+      <c r="I64" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0</v>
+      </c>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="1:7" ht="30">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="3">
+        <v>100</v>
+      </c>
+      <c r="F67" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D61" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -1611,9 +1767,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1631,9 +1787,9 @@
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="B1">
         <v>100</v>
       </c>
@@ -1644,7 +1800,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1660,7 +1816,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="C3" s="7">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
31.03.2025 - Naniesienie szeregu poprawek oraz aktualizacji. Produktywność zaokrąglona do 0 po przecinku; przeniesienie działów między produkcjami; dodanie inwentaryzacji
</commit_message>
<xml_diff>
--- a/#Do zrobienia.xlsx
+++ b/#Do zrobienia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFDE86E-9477-4C8F-852A-2DE66F68ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880CC946-1115-4C79-999F-C83E8AA0368C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="-13230" windowWidth="23490" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Lp</t>
   </si>
@@ -349,6 +349,31 @@
       <t>.
 Dodanie zmiennej przenoszonej do formsa korekty - nowy wpis</t>
     </r>
+  </si>
+  <si>
+    <t>Dodanie okien.
+Sprawdzić możliwość sapisu pracowników w nowych oknach</t>
+  </si>
+  <si>
+    <t>Dodanie plików: transportCzForm, transportCzFormDodaj zarówno szablonów jak i plików z kodem
+Zmiana Menu Ustawienia - dodanie przycisku dla transportuCz
+Dodanie tabeli w bazie - transport produkcji
+Dodanie procedur do bazy danych</t>
+  </si>
+  <si>
+    <t>Ponieważ nie będzie podziału pracowników na pierwszą i drugą zmianęnależy zmienić sposób grupowania linii dla transportu. Przykładem może być grupowani w WC dla liderów. To samo rozwiązanie będzie idealnie pasowało w tym przypadku</t>
+  </si>
+  <si>
+    <t>Dodanie zakładki do wyliczania premii dla Inwentaryzacji.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodano kolumny do tabeli KPI_MAG
+Dodano pozycję w tabeli GRUPY_MAG - na sztywno w programie dodane jest ID - 7. Należy sprawdzić czy nic się nie zmieniło przed kompilacją
+Dodano dane do tabeli WYTYCZNE_MAG - tak naprawde są to 3 pozycje. Należy sprawdzić ID grupy czy jest poprawne z  tym w kodzie. 
+</t>
+  </si>
+  <si>
+    <t>Produktywność dla wszystkich została zaokrąglona do 0 po przecinku</t>
   </si>
 </sst>
 </file>
@@ -447,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -479,6 +504,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -764,11 +795,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -780,6 +811,7 @@
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="115.42578125" customWidth="1"/>
+    <col min="10" max="10" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
@@ -797,15 +829,15 @@
       </c>
       <c r="F1" s="5">
         <f>COUNTA(C2:C199)</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D199)</f>
-        <v>3705</v>
+        <v>4105</v>
       </c>
       <c r="H1" s="4">
         <f>G1/F1</f>
-        <v>56.136363636363633</v>
+        <v>60.367647058823529</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1665,7 +1697,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30">
+    <row r="65" spans="1:10" ht="30">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1676,11 +1708,11 @@
         <v>90</v>
       </c>
       <c r="D65" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:10" ht="67.5" customHeight="1">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1691,11 +1723,22 @@
         <v>91</v>
       </c>
       <c r="D66" s="3">
-        <v>0</v>
-      </c>
-      <c r="F66" s="12"/>
-    </row>
-    <row r="67" spans="1:7" ht="30">
+        <v>100</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J66" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1709,6 +1752,37 @@
         <v>100</v>
       </c>
       <c r="F67" s="13"/>
+    </row>
+    <row r="68" spans="1:10" ht="90">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="3">
+        <v>100</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="3">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D61" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -1721,6 +1795,9 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="E66:H66"/>
+  </mergeCells>
   <conditionalFormatting sqref="D2:D97">
     <cfRule type="dataBar" priority="2">
       <dataBar>

</xml_diff>